<commit_message>
Updates #2 Carrier Regisrer | OOP version
</commit_message>
<xml_diff>
--- a/airport_petty_algorithms/carrier_register_li/Звіт РТ.xlsx
+++ b/airport_petty_algorithms/carrier_register_li/Звіт РТ.xlsx
@@ -601,7 +601,7 @@
       <selection activeCell="C5" sqref="C5:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
     <col width="7.85546875" customWidth="1" style="2" min="1" max="1"/>
     <col width="7" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
@@ -642,7 +642,7 @@
     <row r="3" ht="30" customHeight="1" s="2">
       <c r="B3" s="14" t="inlineStr">
         <is>
-          <t>Дата: 23.08.2021</t>
+          <t>Дата: 24.08.2021</t>
         </is>
       </c>
       <c r="C3" s="20" t="n"/>
@@ -877,7 +877,9 @@
         </is>
       </c>
       <c r="D21" s="21" t="n"/>
-      <c r="E21" s="9" t="n"/>
+      <c r="E21" s="9" t="n">
+        <v>77762</v>
+      </c>
     </row>
     <row r="22" ht="30" customHeight="1" s="2">
       <c r="B22" s="22" t="n"/>
@@ -898,7 +900,7 @@
       </c>
       <c r="D23" s="21" t="n"/>
       <c r="E23" s="9" t="n">
-        <v>500000</v>
+        <v>120000</v>
       </c>
     </row>
     <row r="24" ht="30" customHeight="1" s="2">
@@ -909,7 +911,9 @@
         </is>
       </c>
       <c r="D24" s="21" t="n"/>
-      <c r="E24" s="9" t="n"/>
+      <c r="E24" s="9" t="n">
+        <v>742238</v>
+      </c>
     </row>
     <row r="25" ht="30" customHeight="1" s="2">
       <c r="B25" s="10" t="n"/>
@@ -974,7 +978,7 @@
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
     <col width="8.7109375" customWidth="1" style="2" min="1" max="1024"/>
   </cols>
@@ -996,7 +1000,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="12.75" outlineLevelCol="0"/>
   <cols>
     <col width="8.7109375" customWidth="1" style="2" min="1" max="1024"/>
   </cols>

</xml_diff>